<commit_message>
more more profiling data
</commit_message>
<xml_diff>
--- a/profiling/profile_book.xlsx
+++ b/profiling/profile_book.xlsx
@@ -9,20 +9,24 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" tabRatio="846"/>
   </bookViews>
   <sheets>
     <sheet name="Resultados" sheetId="1" r:id="rId1"/>
-    <sheet name="SIBENIK_V256_R720_S0.5" sheetId="6" r:id="rId2"/>
-    <sheet name="CORNELL_V256_R720_S0.5" sheetId="7" r:id="rId3"/>
-    <sheet name="CONFERENCE_V256_R720_S0.5" sheetId="2" r:id="rId4"/>
-    <sheet name="CONFERENCE_V64_R720_S0.5" sheetId="9" r:id="rId5"/>
-    <sheet name="SPONZA_V256_R720_S0.5" sheetId="3" r:id="rId6"/>
+    <sheet name="SIBENIK_V64_R720_S0.5" sheetId="11" r:id="rId2"/>
+    <sheet name="SIBENIK_V256_R720_S0.5" sheetId="6" r:id="rId3"/>
+    <sheet name="CORNELL_V256_R720_S0.5" sheetId="7" r:id="rId4"/>
+    <sheet name="CORNELL_V64_R720_S0.5" sheetId="10" r:id="rId5"/>
+    <sheet name="CONFERENCE_V256_R720_S0.5" sheetId="2" r:id="rId6"/>
+    <sheet name="CONFERENCE_V64_R720_S0.5" sheetId="9" r:id="rId7"/>
+    <sheet name="SPONZA_V256_R720_S0.5" sheetId="3" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="Conference_V64_R720p_SL05" localSheetId="4">CONFERENCE_V64_R720_S0.5!$A$1:$D$158</definedName>
-    <definedName name="Cornell_V256_R720p_SL05" localSheetId="2">CORNELL_V256_R720_S0.5!$A$1:$D$53</definedName>
-    <definedName name="Sibenik_V256_R720p_SL05" localSheetId="1">SIBENIK_V256_R720_S0.5!$A$1:$D$81</definedName>
+    <definedName name="Conference_V64_R720p_SL05" localSheetId="6">CONFERENCE_V64_R720_S0.5!$A$1:$D$158</definedName>
+    <definedName name="Cornell_V256_R720p_SL05" localSheetId="3">CORNELL_V256_R720_S0.5!$A$1:$D$53</definedName>
+    <definedName name="Cornell_V64_R720p_SL05" localSheetId="4">CORNELL_V64_R720_S0.5!$A$1:$D$49</definedName>
+    <definedName name="Sibenik_V256_R720p_SL05" localSheetId="2">SIBENIK_V256_R720_S0.5!$A$1:$D$81</definedName>
+    <definedName name="Sibenik_V64_R720p_SL05" localSheetId="1">SIBENIK_V64_R720_S0.5!$A$1:$D$77</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -56,8 +60,28 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="Sibenik_V256_R720p_SL05" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="3" name="Cornell_V64_R720p_SL05" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="D:\Documents\Projects\Thesis\profiling\profiles\base_performance\Cornell_V64_R720p_SL05.csv" comma="1">
+      <textFields count="4">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="4" name="Sibenik_V256_R720p_SL05" type="6" refreshedVersion="5" background="1" saveData="1">
     <textPr codePage="437" sourceFile="D:\Documents\Projects\Thesis\profiling\profiles\base_performance\Sibenik_V256_R720p_SL05.csv" tab="0" comma="1">
+      <textFields count="4">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="5" name="Sibenik_V64_R720p_SL05" type="6" refreshedVersion="5" background="1" saveData="1">
+    <textPr codePage="437" sourceFile="D:\Documents\Projects\Thesis\profiling\profiles\base_performance\Sibenik_V64_R720p_SL05.csv" comma="1">
       <textFields count="4">
         <textField/>
         <textField/>
@@ -70,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2893" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3147" uniqueCount="42">
   <si>
     <t>Escena</t>
   </si>
@@ -383,7 +407,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="3" applyAlignment="1">
@@ -412,7 +436,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Cálculo" xfId="3" builtinId="22"/>
@@ -434,14 +457,22 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Sibenik_V256_R720p_SL05" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Sibenik_V64_R720p_SL05" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Sibenik_V256_R720p_SL05" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Cornell_V256_R720p_SL05" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Cornell_V64_R720p_SL05" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Conference_V64_R720p_SL05" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -714,7 +745,7 @@
   <dimension ref="A1:X27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1110,48 +1141,48 @@
         <v>8</v>
       </c>
       <c r="C13" s="15">
-        <f>SUM(CORNELL_V256_R720_S0.5!C3:C15)</f>
-        <v>0.99333500000000008</v>
+        <f>SUM(CORNELL_V64_R720_S0.5!C3:C15)</f>
+        <v>0.95837100000000008</v>
       </c>
       <c r="D13" s="15">
-        <f>SUM(CORNELL_V256_R720_S0.5!C16:C20)</f>
-        <v>0.50785199999999997</v>
+        <f>SUM(CORNELL_V64_R720_S0.5!C16:C20)</f>
+        <v>6.785200000000001E-2</v>
       </c>
       <c r="E13" s="16">
-        <f>SUM(CORNELL_V256_R720_S0.5!C21)</f>
-        <v>0.78014799999999995</v>
+        <f>SUM(CORNELL_V64_R720_S0.5!C21)</f>
+        <v>2.0445000000000001E-2</v>
       </c>
       <c r="F13" s="15">
-        <f>SUM(CORNELL_V256_R720_S0.5!C22:C25)</f>
-        <v>1.3047410000000002</v>
+        <f>SUM(CORNELL_V64_R720_S0.5!C22:C25)</f>
+        <v>2.1337790000000001</v>
       </c>
       <c r="G13" s="15">
-        <f>SUM(CORNELL_V256_R720_S0.5!C26)</f>
-        <v>1.3348199999999999</v>
+        <f>SUM(CORNELL_V64_R720_S0.5!C26)</f>
+        <v>6.4445000000000002E-2</v>
       </c>
       <c r="H13" s="15">
-        <f>SUM(CORNELL_V256_R720_S0.5!C27:C34)</f>
-        <v>1.3752609999999998</v>
+        <f>SUM(CORNELL_V64_R720_S0.5!C27:C32)</f>
+        <v>0.10577700000000001</v>
       </c>
       <c r="I13" s="15">
-        <f>SUM(CORNELL_V256_R720_S0.5!C35)</f>
-        <v>8.4124400000000001</v>
+        <f>SUM(CORNELL_V64_R720_S0.5!C33)</f>
+        <v>0.288296</v>
       </c>
       <c r="J13" s="15">
-        <f>SUM(CORNELL_V256_R720_S0.5!C36:C43)</f>
-        <v>1.3724449999999997</v>
+        <f>SUM(CORNELL_V64_R720_S0.5!C34:C39)</f>
+        <v>0.105185</v>
       </c>
       <c r="K13" s="15">
-        <f>SUM(CORNELL_V256_R720_S0.5!C44:C51)</f>
-        <v>0.63214800000000004</v>
+        <f>SUM(CORNELL_V64_R720_S0.5!C40:C47)</f>
+        <v>0.61199999999999988</v>
       </c>
       <c r="L13" s="15">
-        <f>SUM(CORNELL_V256_R720_S0.5!C52:C53)</f>
-        <v>7.2259220000000006</v>
+        <f>SUM(CORNELL_V64_R720_S0.5!C48:C49)</f>
+        <v>4.7934850000000004</v>
       </c>
       <c r="M13" s="15">
         <f t="shared" si="0"/>
-        <v>23.939112000000002</v>
+        <v>9.149635</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
@@ -1479,7 +1510,7 @@
         <f>SUM(SIBENIK_V256_R720_S0.5!C46:C49)</f>
         <v>2.1134859999999995</v>
       </c>
-      <c r="G20" s="20">
+      <c r="G20" s="16">
         <f>SUM(SIBENIK_V256_R720_S0.5!C50)</f>
         <v>0.94681499999999996</v>
       </c>
@@ -1873,6 +1904,1100 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D77"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="81.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>75</v>
+      </c>
+      <c r="C2">
+        <v>19.540732999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1.4666E-2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>0.112888</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>1.8814000000000001E-2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>1.4899999999999999E-4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>1.9407000000000001E-2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>1.4809999999999999E-3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>2.9700000000000001E-4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>1.4799999999999999E-4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>8.1480000000000007E-3</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>6.9037000000000001E-2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>1.0963000000000001E-2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15">
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <v>4.7406999999999998E-2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>2.3709999999999998E-3</v>
+      </c>
+      <c r="D16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <v>3.555E-3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19">
+        <v>17</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>18</v>
+      </c>
+      <c r="C20">
+        <v>6.0740000000000004E-3</v>
+      </c>
+      <c r="D20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>19</v>
+      </c>
+      <c r="C21">
+        <v>5.7630000000000001E-2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>20</v>
+      </c>
+      <c r="C22">
+        <v>6.0593000000000001E-2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23">
+        <v>21</v>
+      </c>
+      <c r="C23">
+        <v>1.4814000000000001E-2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24">
+        <v>22</v>
+      </c>
+      <c r="C24">
+        <v>0.106963</v>
+      </c>
+      <c r="D24" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25">
+        <v>23</v>
+      </c>
+      <c r="C25">
+        <v>0.14918500000000001</v>
+      </c>
+      <c r="D25" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26">
+        <v>24</v>
+      </c>
+      <c r="C26">
+        <v>9.5407000000000006E-2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27">
+        <v>25</v>
+      </c>
+      <c r="C27">
+        <v>0.14711099999999999</v>
+      </c>
+      <c r="D27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28">
+        <v>26</v>
+      </c>
+      <c r="C28">
+        <v>6.8149999999999999E-3</v>
+      </c>
+      <c r="D28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29">
+        <v>27</v>
+      </c>
+      <c r="C29">
+        <v>0.11688900000000001</v>
+      </c>
+      <c r="D29" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30">
+        <v>28</v>
+      </c>
+      <c r="C30">
+        <v>8.9926000000000006E-2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31">
+        <v>29</v>
+      </c>
+      <c r="C31">
+        <v>5.9199999999999997E-4</v>
+      </c>
+      <c r="D31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32">
+        <v>30</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33">
+        <v>31</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B34">
+        <v>32</v>
+      </c>
+      <c r="C34">
+        <v>2.4740000000000002E-2</v>
+      </c>
+      <c r="D34" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35">
+        <v>33</v>
+      </c>
+      <c r="C35">
+        <v>2.6670000000000001E-3</v>
+      </c>
+      <c r="D35" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36">
+        <v>34</v>
+      </c>
+      <c r="C36">
+        <v>1.4799999999999999E-4</v>
+      </c>
+      <c r="D36" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37">
+        <v>35</v>
+      </c>
+      <c r="C37">
+        <v>0.23511099999999999</v>
+      </c>
+      <c r="D37" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38">
+        <v>36</v>
+      </c>
+      <c r="C38">
+        <v>0.87703699999999996</v>
+      </c>
+      <c r="D38" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>20</v>
+      </c>
+      <c r="B39">
+        <v>37</v>
+      </c>
+      <c r="C39">
+        <v>0.93185200000000001</v>
+      </c>
+      <c r="D39" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40">
+        <v>38</v>
+      </c>
+      <c r="C40">
+        <v>0.385185</v>
+      </c>
+      <c r="D40" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41">
+        <v>39</v>
+      </c>
+      <c r="C41">
+        <v>1.4799999999999999E-4</v>
+      </c>
+      <c r="D41" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>20</v>
+      </c>
+      <c r="B42">
+        <v>40</v>
+      </c>
+      <c r="C42">
+        <v>5.9299999999999999E-4</v>
+      </c>
+      <c r="D42" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>20</v>
+      </c>
+      <c r="B43">
+        <v>41</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>20</v>
+      </c>
+      <c r="B44">
+        <v>42</v>
+      </c>
+      <c r="C44">
+        <v>0.32859300000000002</v>
+      </c>
+      <c r="D44" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>27</v>
+      </c>
+      <c r="B45">
+        <v>43</v>
+      </c>
+      <c r="C45">
+        <v>1.3481E-2</v>
+      </c>
+      <c r="D45" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>17</v>
+      </c>
+      <c r="B46">
+        <v>44</v>
+      </c>
+      <c r="C46">
+        <v>6.3709999999999999E-3</v>
+      </c>
+      <c r="D46" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>20</v>
+      </c>
+      <c r="B47">
+        <v>45</v>
+      </c>
+      <c r="C47">
+        <v>5.5765900000000004</v>
+      </c>
+      <c r="D47" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>20</v>
+      </c>
+      <c r="B48">
+        <v>46</v>
+      </c>
+      <c r="C48">
+        <v>3.0456300000000001</v>
+      </c>
+      <c r="D48" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>20</v>
+      </c>
+      <c r="B49">
+        <v>47</v>
+      </c>
+      <c r="C49">
+        <v>0.54237000000000002</v>
+      </c>
+      <c r="D49" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>27</v>
+      </c>
+      <c r="B50">
+        <v>48</v>
+      </c>
+      <c r="C50">
+        <v>4.2369999999999998E-2</v>
+      </c>
+      <c r="D50" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>27</v>
+      </c>
+      <c r="B51">
+        <v>49</v>
+      </c>
+      <c r="C51">
+        <v>2.0889000000000001E-2</v>
+      </c>
+      <c r="D51" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>27</v>
+      </c>
+      <c r="B52">
+        <v>50</v>
+      </c>
+      <c r="C52">
+        <v>2.0740000000000001E-2</v>
+      </c>
+      <c r="D52" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>27</v>
+      </c>
+      <c r="B53">
+        <v>51</v>
+      </c>
+      <c r="C53">
+        <v>1.9554999999999999E-2</v>
+      </c>
+      <c r="D53" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>27</v>
+      </c>
+      <c r="B54">
+        <v>52</v>
+      </c>
+      <c r="C54">
+        <v>1.6593E-2</v>
+      </c>
+      <c r="D54" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>27</v>
+      </c>
+      <c r="B55">
+        <v>53</v>
+      </c>
+      <c r="C55">
+        <v>1.4815E-2</v>
+      </c>
+      <c r="D55" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>27</v>
+      </c>
+      <c r="B56">
+        <v>54</v>
+      </c>
+      <c r="C56">
+        <v>1.4963000000000001E-2</v>
+      </c>
+      <c r="D56" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>27</v>
+      </c>
+      <c r="B57">
+        <v>55</v>
+      </c>
+      <c r="C57">
+        <v>0.123852</v>
+      </c>
+      <c r="D57" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>27</v>
+      </c>
+      <c r="B58">
+        <v>56</v>
+      </c>
+      <c r="C58">
+        <v>2.0593E-2</v>
+      </c>
+      <c r="D58" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>27</v>
+      </c>
+      <c r="B59">
+        <v>57</v>
+      </c>
+      <c r="C59">
+        <v>2.1184999999999999E-2</v>
+      </c>
+      <c r="D59" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>27</v>
+      </c>
+      <c r="B60">
+        <v>58</v>
+      </c>
+      <c r="C60">
+        <v>1.8223E-2</v>
+      </c>
+      <c r="D60" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>27</v>
+      </c>
+      <c r="B61">
+        <v>59</v>
+      </c>
+      <c r="C61">
+        <v>1.5407000000000001E-2</v>
+      </c>
+      <c r="D61" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>27</v>
+      </c>
+      <c r="B62">
+        <v>60</v>
+      </c>
+      <c r="C62">
+        <v>1.4815E-2</v>
+      </c>
+      <c r="D62" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>27</v>
+      </c>
+      <c r="B63">
+        <v>61</v>
+      </c>
+      <c r="C63">
+        <v>1.4519000000000001E-2</v>
+      </c>
+      <c r="D63" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>17</v>
+      </c>
+      <c r="B64">
+        <v>62</v>
+      </c>
+      <c r="C64">
+        <v>0.14888899999999999</v>
+      </c>
+      <c r="D64" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>20</v>
+      </c>
+      <c r="B65">
+        <v>63</v>
+      </c>
+      <c r="C65">
+        <v>1.4666999999999999E-2</v>
+      </c>
+      <c r="D65" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>20</v>
+      </c>
+      <c r="B66">
+        <v>64</v>
+      </c>
+      <c r="C66">
+        <v>1.2444E-2</v>
+      </c>
+      <c r="D66" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>20</v>
+      </c>
+      <c r="B67">
+        <v>65</v>
+      </c>
+      <c r="C67">
+        <v>3.4222000000000002E-2</v>
+      </c>
+      <c r="D67" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>20</v>
+      </c>
+      <c r="B68">
+        <v>66</v>
+      </c>
+      <c r="C68">
+        <v>1.3481999999999999E-2</v>
+      </c>
+      <c r="D68" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>20</v>
+      </c>
+      <c r="B69">
+        <v>67</v>
+      </c>
+      <c r="C69">
+        <v>1.6E-2</v>
+      </c>
+      <c r="D69" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>20</v>
+      </c>
+      <c r="B70">
+        <v>68</v>
+      </c>
+      <c r="C70">
+        <v>0.30088900000000002</v>
+      </c>
+      <c r="D70" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>20</v>
+      </c>
+      <c r="B71">
+        <v>69</v>
+      </c>
+      <c r="C71">
+        <v>1.1850000000000001E-3</v>
+      </c>
+      <c r="D71" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>20</v>
+      </c>
+      <c r="B72">
+        <v>70</v>
+      </c>
+      <c r="C72">
+        <v>6.5180000000000004E-3</v>
+      </c>
+      <c r="D72" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>20</v>
+      </c>
+      <c r="B73">
+        <v>71</v>
+      </c>
+      <c r="C73">
+        <v>0.118074</v>
+      </c>
+      <c r="D73" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>20</v>
+      </c>
+      <c r="B74">
+        <v>72</v>
+      </c>
+      <c r="C74">
+        <v>0.112148</v>
+      </c>
+      <c r="D74" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>20</v>
+      </c>
+      <c r="B75">
+        <v>73</v>
+      </c>
+      <c r="C75">
+        <v>7.7925999999999995E-2</v>
+      </c>
+      <c r="D75" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>17</v>
+      </c>
+      <c r="B76">
+        <v>74</v>
+      </c>
+      <c r="C76">
+        <v>1.4074E-2</v>
+      </c>
+      <c r="D76" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>20</v>
+      </c>
+      <c r="B77">
+        <v>75</v>
+      </c>
+      <c r="C77">
+        <v>5.1598499999999996</v>
+      </c>
+      <c r="D77" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D81"/>
   <sheetViews>
@@ -3022,11 +4147,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A15" workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
@@ -3782,7 +4907,711 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D49"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="81.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>47</v>
+      </c>
+      <c r="C2">
+        <v>9.149635</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1.8221999999999999E-2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>0.112889</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>0.11407399999999999</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>7.4079999999999997E-3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>2.9599999999999998E-4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>2.5777999999999999E-2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>5.8666000000000003E-2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>6.2222E-2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>1.7186E-2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>0.106222</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>11</v>
+      </c>
+      <c r="C13">
+        <v>0.17125899999999999</v>
+      </c>
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>12</v>
+      </c>
+      <c r="C14">
+        <v>9.4814999999999997E-2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15">
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <v>0.16933400000000001</v>
+      </c>
+      <c r="D15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>6.9629999999999996E-3</v>
+      </c>
+      <c r="D16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>6.0297000000000003E-2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>16</v>
+      </c>
+      <c r="C18">
+        <v>2.9599999999999998E-4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19">
+        <v>17</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>18</v>
+      </c>
+      <c r="C20">
+        <v>2.9599999999999998E-4</v>
+      </c>
+      <c r="D20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21">
+        <v>19</v>
+      </c>
+      <c r="C21">
+        <v>2.0445000000000001E-2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22">
+        <v>20</v>
+      </c>
+      <c r="C22">
+        <v>6.2220000000000001E-3</v>
+      </c>
+      <c r="D22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23">
+        <v>21</v>
+      </c>
+      <c r="C23">
+        <v>0.98518600000000001</v>
+      </c>
+      <c r="D23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24">
+        <v>22</v>
+      </c>
+      <c r="C24">
+        <v>1.0392600000000001</v>
+      </c>
+      <c r="D24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25">
+        <v>23</v>
+      </c>
+      <c r="C25">
+        <v>0.10311099999999999</v>
+      </c>
+      <c r="D25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26">
+        <v>24</v>
+      </c>
+      <c r="C26">
+        <v>6.4445000000000002E-2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27">
+        <v>25</v>
+      </c>
+      <c r="C27">
+        <v>2.2519000000000001E-2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>26</v>
+      </c>
+      <c r="C28">
+        <v>2.0740000000000001E-2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>27</v>
+      </c>
+      <c r="C29">
+        <v>1.8518E-2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30">
+        <v>28</v>
+      </c>
+      <c r="C30">
+        <v>1.5259E-2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31">
+        <v>29</v>
+      </c>
+      <c r="C31">
+        <v>1.4370000000000001E-2</v>
+      </c>
+      <c r="D31" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32">
+        <v>30</v>
+      </c>
+      <c r="C32">
+        <v>1.4371E-2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33">
+        <v>31</v>
+      </c>
+      <c r="C33">
+        <v>0.288296</v>
+      </c>
+      <c r="D33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>27</v>
+      </c>
+      <c r="B34">
+        <v>32</v>
+      </c>
+      <c r="C34">
+        <v>2.1777999999999999E-2</v>
+      </c>
+      <c r="D34" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>27</v>
+      </c>
+      <c r="B35">
+        <v>33</v>
+      </c>
+      <c r="C35">
+        <v>2.0740999999999999E-2</v>
+      </c>
+      <c r="D35" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>27</v>
+      </c>
+      <c r="B36">
+        <v>34</v>
+      </c>
+      <c r="C36">
+        <v>1.8519000000000001E-2</v>
+      </c>
+      <c r="D36" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37">
+        <v>35</v>
+      </c>
+      <c r="C37">
+        <v>1.5407000000000001E-2</v>
+      </c>
+      <c r="D37" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>27</v>
+      </c>
+      <c r="B38">
+        <v>36</v>
+      </c>
+      <c r="C38">
+        <v>1.4666E-2</v>
+      </c>
+      <c r="D38" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39">
+        <v>37</v>
+      </c>
+      <c r="C39">
+        <v>1.4074E-2</v>
+      </c>
+      <c r="D39" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>17</v>
+      </c>
+      <c r="B40">
+        <v>38</v>
+      </c>
+      <c r="C40">
+        <v>0.14888899999999999</v>
+      </c>
+      <c r="D40" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41">
+        <v>39</v>
+      </c>
+      <c r="C41">
+        <v>0.104</v>
+      </c>
+      <c r="D41" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>20</v>
+      </c>
+      <c r="B42">
+        <v>40</v>
+      </c>
+      <c r="C42">
+        <v>4.2666000000000003E-2</v>
+      </c>
+      <c r="D42" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>20</v>
+      </c>
+      <c r="B43">
+        <v>41</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>20</v>
+      </c>
+      <c r="B44">
+        <v>42</v>
+      </c>
+      <c r="C44">
+        <v>4.5185999999999997E-2</v>
+      </c>
+      <c r="D44" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>20</v>
+      </c>
+      <c r="B45">
+        <v>43</v>
+      </c>
+      <c r="C45">
+        <v>0.14014799999999999</v>
+      </c>
+      <c r="D45" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>20</v>
+      </c>
+      <c r="B46">
+        <v>44</v>
+      </c>
+      <c r="C46">
+        <v>9.2147999999999994E-2</v>
+      </c>
+      <c r="D46" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>20</v>
+      </c>
+      <c r="B47">
+        <v>45</v>
+      </c>
+      <c r="C47">
+        <v>3.8962999999999998E-2</v>
+      </c>
+      <c r="D47" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>17</v>
+      </c>
+      <c r="B48">
+        <v>46</v>
+      </c>
+      <c r="C48">
+        <v>1.3185000000000001E-2</v>
+      </c>
+      <c r="D48" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>20</v>
+      </c>
+      <c r="B49">
+        <v>47</v>
+      </c>
+      <c r="C49">
+        <v>4.7803000000000004</v>
+      </c>
+      <c r="D49" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -6066,7 +7895,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D158"/>
   <sheetViews>
@@ -8296,7 +10125,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D967"/>
   <sheetViews>

</xml_diff>